<commit_message>
dataCollecttion : rename columns of peace indicator + compliledata : reorganize code + outputs
</commit_message>
<xml_diff>
--- a/Output/regression.xlsx
+++ b/Output/regression.xlsx
@@ -818,7 +818,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Global_Peace_Index 2023</t>
+          <t>Global Peace Index 2023</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Poverty headcount ratio at $6.85 a day (% of population)</t>
+          <t>Poverty $6.85 a day (% of population)</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -998,7 +998,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ease of doing business score</t>
+          <t>doing business score</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Armed forces (% of total labor force)</t>
+          <t>Armed forces (% labor force)</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>corruption index 2023</t>
+          <t>Corruption index 2023</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Poverty headcount ratio at $3.65 a day (% of population)</t>
+          <t>Poverty $3.65 a day (% of population)</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Poverty headcount ratio at $2.15 a day (% of population)</t>
+          <t>Poverty $2.15 a day (% of population)</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Unemployment  advanced education</t>
+          <t>Unemployment advanced education</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Time required to start a business (days)</t>
+          <t>Time to start a business (days)</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>GNI per capita (constant 2015 US$)</t>
+          <t>GNI per capita (2015 US$)</t>
         </is>
       </c>
       <c r="E48" t="n">

</xml_diff>